<commit_message>
Completed Software Benchmarking for Matrix Multiplication
- Finished writing the code to the CuPy version of matrix multiplication
- Outputted results to excel and image file
- comparison can be made regarding NumPy and CuPy (CPU vs GPU) and written as a report in the readme file.
</commit_message>
<xml_diff>
--- a/Software Benchmarking - Matrix Multiplication/numpy_float_matrix_mult.xlsx
+++ b/Software Benchmarking - Matrix Multiplication/numpy_float_matrix_mult.xlsx
@@ -396,7 +396,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5.245208740234375E-06</v>
+        <v>5.483627319335938E-06</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -404,7 +404,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>3.767013549804688E-05</v>
+        <v>3.862380981445312E-05</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -412,7 +412,7 @@
         <v>100</v>
       </c>
       <c r="B4">
-        <v>0.0003652572631835938</v>
+        <v>0.0001327991485595703</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -420,7 +420,7 @@
         <v>500</v>
       </c>
       <c r="B5">
-        <v>0.003241539001464844</v>
+        <v>0.003339290618896484</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -428,7 +428,7 @@
         <v>1000</v>
       </c>
       <c r="B6">
-        <v>0.01163983345031738</v>
+        <v>0.01249885559082031</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -436,7 +436,7 @@
         <v>1500</v>
       </c>
       <c r="B7">
-        <v>0.0333092212677002</v>
+        <v>0.05233240127563477</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -444,7 +444,7 @@
         <v>2000</v>
       </c>
       <c r="B8">
-        <v>0.0716698169708252</v>
+        <v>0.07263898849487305</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -452,7 +452,7 @@
         <v>3500</v>
       </c>
       <c r="B9">
-        <v>0.3498895168304443</v>
+        <v>0.3523106575012207</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -460,7 +460,7 @@
         <v>5000</v>
       </c>
       <c r="B10">
-        <v>0.9535071849822998</v>
+        <v>0.9420583248138428</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -468,7 +468,7 @@
         <v>7500</v>
       </c>
       <c r="B11">
-        <v>3.082071781158447</v>
+        <v>3.11338210105896</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -476,7 +476,7 @@
         <v>10000</v>
       </c>
       <c r="B12">
-        <v>6.933080434799194</v>
+        <v>7.020748376846313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>